<commit_message>
Added RelayControls to use child clicks to fire parent command Realised I could do the same thing wit IsHitTestVisible in the xaml
</commit_message>
<xml_diff>
--- a/xamlLoaderCodePath.xlsx
+++ b/xamlLoaderCodePath.xlsx
@@ -10,8 +10,6 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="9780" activeTab="1"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9780" firstSheet="2" activeTab="5"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14310" windowHeight="9780" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="408">
   <si>
     <t>PresentationFramework.dll!System.Windows.EventSetter.Event.set(System.Windows.RoutedEvent value) Line 30</t>
   </si>
@@ -1253,6 +1251,9 @@
   </si>
   <si>
     <t>PresentationCore.dll!System.Windows.UIElement.RaiseEventImpl(System.Windows.DependencyObject sender, System.Windows.RoutedEventArgs args) Line 6120</t>
+  </si>
+  <si>
+    <t>inst = EventSetter, property = Event, value = RoutedEvent Click</t>
   </si>
 </sst>
 </file>
@@ -1294,81 +1295,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1422,16 +1355,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -1444,49 +1367,14 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1803,8 +1691,6 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2966,10 +2852,6 @@
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
-    <sheetView topLeftCell="B1" workbookViewId="1">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4114,10 +3996,6 @@
     <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
-    <sheetView topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5265,8 +5143,6 @@
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8395,10 +8271,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-    <sheetView workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8445,16 +8317,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C79"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="2">
-      <selection sqref="A1:A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8463,7 +8329,7 @@
     <col min="6" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>ROW()</f>
         <v>1</v>
@@ -8476,27 +8342,27 @@
         <v>0</v>
       </c>
       <c r="E1" t="str">
-        <f>RIGHT(D1,LEN(D1)-FIND("Line ",D1)+1)</f>
+        <f t="shared" ref="E1:E32" si="0">RIGHT(D1,LEN(D1)-FIND("Line ",D1)+1)</f>
         <v>Line 30</v>
       </c>
       <c r="F1" t="str">
-        <f>LEFT(D1,LEN(D1)-LEN(E1))</f>
+        <f t="shared" ref="F1:F32" si="1">LEFT(D1,LEN(D1)-LEN(E1))</f>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.EventSetter.Event.set(System.Windows.RoutedEvent value) </v>
       </c>
       <c r="G1" t="str">
-        <f>LEFT(F1,FIND("(",F1))</f>
+        <f t="shared" ref="G1:G32" si="2">LEFT(F1,FIND("(",F1))</f>
         <v>PresentationFramework.dll!System.Windows.EventSetter.Event.set(</v>
       </c>
       <c r="H1">
-        <f>FIND("@",SUBSTITUTE(G1,".","@",LEN(G1)-LEN(SUBSTITUTE(G1,".",""))))</f>
+        <f t="shared" ref="H1:H32" si="3">FIND("@",SUBSTITUTE(G1,".","@",LEN(G1)-LEN(SUBSTITUTE(G1,".",""))))</f>
         <v>59</v>
       </c>
       <c r="I1" t="str">
-        <f>RIGHT(F1,LEN(F1)-H1)</f>
+        <f t="shared" ref="I1:I32" si="4">RIGHT(F1,LEN(F1)-H1)</f>
         <v xml:space="preserve">set(System.Windows.RoutedEvent value) </v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>C1+1</f>
         <v>2</v>
@@ -8505,2571 +8371,2574 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C65" si="0">$A2-B2</f>
+        <f t="shared" ref="C2:C65" si="5">$A2-B2</f>
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="e">
-        <f>RIGHT(D2,LEN(D2)-FIND("Line ",D2)+1)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="F2" t="e">
-        <f>LEFT(D2,LEN(D2)-LEN(E2))</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="G2" t="e">
-        <f>LEFT(F2,FIND("(",F2))</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="H2" t="e">
-        <f>FIND("@",SUBSTITUTE(G2,".","@",LEN(G2)-LEN(SUBSTITUTE(G2,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I2" t="e">
-        <f>RIGHT(F2,LEN(F2)-H2)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A66" si="1">C2+1</f>
+        <f t="shared" ref="A3:A66" si="6">C2+1</f>
         <v>3</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="E3" t="e">
-        <f>RIGHT(D3,LEN(D3)-FIND("Line ",D3)+1)</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="F3" t="e">
-        <f>LEFT(D3,LEN(D3)-LEN(E3))</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="G3" t="e">
-        <f>LEFT(F3,FIND("(",F3))</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="H3" t="e">
-        <f>FIND("@",SUBSTITUTE(G3,".","@",LEN(G3)-LEN(SUBSTITUTE(G3,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="I3" t="e">
-        <f>RIGHT(F3,LEN(F3)-H3)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="str">
-        <f>RIGHT(D4,LEN(D4)-FIND("Line ",D4)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 214</v>
       </c>
       <c r="F4" t="str">
-        <f>LEFT(D4,LEN(D4)-LEN(E4))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.InvokeMethodCritical(System.Reflection.MethodInfo method, object instance, object[] args) </v>
       </c>
       <c r="G4" t="str">
-        <f>LEFT(F4,FIND("(",F4))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.InvokeMethodCritical(</v>
       </c>
       <c r="H4">
-        <f>FIND("@",SUBSTITUTE(G4,".","@",LEN(G4)-LEN(SUBSTITUTE(G4,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="I4" t="str">
-        <f>RIGHT(F4,LEN(F4)-H4)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">InvokeMethodCritical(System.Reflection.MethodInfo method, object instance, object[] args) </v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>358</v>
       </c>
       <c r="E5" t="str">
-        <f>RIGHT(D5,LEN(D5)-FIND("Line ",D5)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 208</v>
       </c>
       <c r="F5" t="str">
-        <f>LEFT(D5,LEN(D5)-LEN(E5))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.InvokeMethod(System.Reflection.MethodInfo method, object instance, object[] args) </v>
       </c>
       <c r="G5" t="str">
-        <f>LEFT(F5,FIND("(",F5))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.InvokeMethod(</v>
       </c>
       <c r="H5">
-        <f>FIND("@",SUBSTITUTE(G5,".","@",LEN(G5)-LEN(SUBSTITUTE(G5,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="I5" t="str">
-        <f>RIGHT(F5,LEN(F5)-H5)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">InvokeMethod(System.Reflection.MethodInfo method, object instance, object[] args) </v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>359</v>
       </c>
       <c r="E6" t="str">
-        <f>RIGHT(D6,LEN(D6)-FIND("Line ",D6)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 143</v>
       </c>
       <c r="F6" t="str">
-        <f>LEFT(D6,LEN(D6)-LEN(E6))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.XamlMemberInvoker.SetValueSafeCritical(object instance, object value) </v>
       </c>
       <c r="G6" t="str">
-        <f>LEFT(F6,FIND("(",F6))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.Schema.XamlMemberInvoker.SetValueSafeCritical(</v>
       </c>
       <c r="H6">
-        <f>FIND("@",SUBSTITUTE(G6,".","@",LEN(G6)-LEN(SUBSTITUTE(G6,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="I6" t="str">
-        <f>RIGHT(F6,LEN(F6)-H6)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">SetValueSafeCritical(object instance, object value) </v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>360</v>
       </c>
       <c r="E7" t="str">
-        <f>RIGHT(D7,LEN(D7)-FIND("Line ",D7)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 130</v>
       </c>
       <c r="F7" t="str">
-        <f>LEFT(D7,LEN(D7)-LEN(E7))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.XamlMemberInvoker.SetValue(object instance, object value) </v>
       </c>
       <c r="G7" t="str">
-        <f>LEFT(F7,FIND("(",F7))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.Schema.XamlMemberInvoker.SetValue(</v>
       </c>
       <c r="H7">
-        <f>FIND("@",SUBSTITUTE(G7,".","@",LEN(G7)-LEN(SUBSTITUTE(G7,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>53</v>
       </c>
       <c r="I7" t="str">
-        <f>RIGHT(F7,LEN(F7)-H7)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">SetValue(object instance, object value) </v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>361</v>
       </c>
       <c r="E8" t="str">
-        <f>RIGHT(D8,LEN(D8)-FIND("Line ",D8)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 258</v>
       </c>
       <c r="F8" t="str">
-        <f>LEFT(D8,LEN(D8)-LEN(E8))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.SetValue(System.Xaml.XamlMember member, object obj, object value) </v>
       </c>
       <c r="G8" t="str">
-        <f>LEFT(F8,FIND("(",F8))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.SetValue(</v>
       </c>
       <c r="H8">
-        <f>FIND("@",SUBSTITUTE(G8,".","@",LEN(G8)-LEN(SUBSTITUTE(G8,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="I8" t="str">
-        <f>RIGHT(F8,LEN(F8)-H8)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">SetValue(System.Xaml.XamlMember member, object obj, object value) </v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="str">
-        <f>RIGHT(D9,LEN(D9)-FIND("Line ",D9)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 245</v>
       </c>
       <c r="F9" t="str">
-        <f>LEFT(D9,LEN(D9)-LEN(E9))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.SetValue(object inst, System.Xaml.XamlMember property, object value) </v>
       </c>
       <c r="G9" t="str">
-        <f>LEFT(F9,FIND("(",F9))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.SetValue(</v>
       </c>
       <c r="H9">
-        <f>FIND("@",SUBSTITUTE(G9,".","@",LEN(G9)-LEN(SUBSTITUTE(G9,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="I9" t="str">
-        <f>RIGHT(F9,LEN(F9)-H9)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">SetValue(object inst, System.Xaml.XamlMember property, object value) </v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10" t="str">
-        <f>RIGHT(D10,LEN(D10)-FIND("Line ",D10)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 1123</v>
       </c>
       <c r="F10" t="str">
-        <f>LEFT(D10,LEN(D10)-LEN(E10))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_ApplyPropertyValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx, System.Xaml.XamlMember prop, object value, bool onParent) </v>
       </c>
       <c r="G10" t="str">
-        <f>LEFT(F10,FIND("(",F10))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_ApplyPropertyValue(</v>
       </c>
       <c r="H10">
-        <f>FIND("@",SUBSTITUTE(G10,".","@",LEN(G10)-LEN(SUBSTITUTE(G10,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I10" t="str">
-        <f>RIGHT(F10,LEN(F10)-H10)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Logic_ApplyPropertyValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx, System.Xaml.XamlMember prop, object value, bool onParent) </v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="str">
-        <f>RIGHT(D11,LEN(D11)-FIND("Line ",D11)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 1356</v>
       </c>
       <c r="F11" t="str">
-        <f>LEFT(D11,LEN(D11)-LEN(E11))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_DoAssignmentToParentProperty(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
       <c r="G11" t="str">
-        <f>LEFT(F11,FIND("(",F11))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_DoAssignmentToParentProperty(</v>
       </c>
       <c r="H11">
-        <f>FIND("@",SUBSTITUTE(G11,".","@",LEN(G11)-LEN(SUBSTITUTE(G11,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I11" t="str">
-        <f>RIGHT(F11,LEN(F11)-H11)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Logic_DoAssignmentToParentProperty(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="str">
-        <f>RIGHT(D12,LEN(D12)-FIND("Line ",D12)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 1137</v>
       </c>
       <c r="F12" t="str">
-        <f>LEFT(D12,LEN(D12)-LEN(E12))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_AssignProvidedValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
       <c r="G12" t="str">
-        <f>LEFT(F12,FIND("(",F12))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_AssignProvidedValue(</v>
       </c>
       <c r="H12">
-        <f>FIND("@",SUBSTITUTE(G12,".","@",LEN(G12)-LEN(SUBSTITUTE(G12,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I12" t="str">
-        <f>RIGHT(F12,LEN(F12)-H12)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Logic_AssignProvidedValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="str">
-        <f>RIGHT(D13,LEN(D13)-FIND("Line ",D13)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 577</v>
       </c>
       <c r="F13" t="str">
-        <f>LEFT(D13,LEN(D13)-LEN(E13))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteEndMember() </v>
       </c>
       <c r="G13" t="str">
-        <f>LEFT(F13,FIND("(",F13))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteEndMember(</v>
       </c>
       <c r="H13">
-        <f>FIND("@",SUBSTITUTE(G13,".","@",LEN(G13)-LEN(SUBSTITUTE(G13,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I13" t="str">
-        <f>RIGHT(F13,LEN(F13)-H13)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">WriteEndMember() </v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D14" t="s">
         <v>362</v>
       </c>
       <c r="E14" t="str">
-        <f>RIGHT(D14,LEN(D14)-FIND("Line ",D14)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 72</v>
       </c>
       <c r="F14" t="str">
-        <f>LEFT(D14,LEN(D14)-LEN(E14))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
       <c r="G14" t="str">
-        <f>LEFT(F14,FIND("(",F14))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(</v>
       </c>
       <c r="H14">
-        <f>FIND("@",SUBSTITUTE(G14,".","@",LEN(G14)-LEN(SUBSTITUTE(G14,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="I14" t="str">
-        <f>RIGHT(F14,LEN(F14)-H14)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="str">
-        <f>RIGHT(D15,LEN(D15)-FIND("Line ",D15)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 229</v>
       </c>
       <c r="F15" t="str">
-        <f>LEFT(D15,LEN(D15)-LEN(E15))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
       <c r="G15" t="str">
-        <f>LEFT(F15,FIND("(",F15))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(</v>
       </c>
       <c r="H15">
-        <f>FIND("@",SUBSTITUTE(G15,".","@",LEN(G15)-LEN(SUBSTITUTE(G15,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="I15" t="str">
-        <f>RIGHT(F15,LEN(F15)-H15)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="str">
-        <f>RIGHT(D16,LEN(D16)-FIND("Line ",D16)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 105</v>
       </c>
       <c r="F16" t="str">
-        <f>LEFT(D16,LEN(D16)-LEN(E16))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
       <c r="G16" t="str">
-        <f>LEFT(F16,FIND("(",F16))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(</v>
       </c>
       <c r="H16">
-        <f>FIND("@",SUBSTITUTE(G16,".","@",LEN(G16)-LEN(SUBSTITUTE(G16,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="I16" t="str">
-        <f>RIGHT(F16,LEN(F16)-H16)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>363</v>
       </c>
       <c r="E17" t="str">
-        <f>RIGHT(D17,LEN(D17)-FIND("Line ",D17)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 34</v>
       </c>
       <c r="F17" t="str">
-        <f>LEFT(D17,LEN(D17)-LEN(E17))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadDeferredContent(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings parentSettings, System.Uri baseUri) </v>
       </c>
       <c r="G17" t="str">
-        <f>LEFT(F17,FIND("(",F17))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadDeferredContent(</v>
       </c>
       <c r="H17">
-        <f>FIND("@",SUBSTITUTE(G17,".","@",LEN(G17)-LEN(SUBSTITUTE(G17,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="I17" t="str">
-        <f>RIGHT(F17,LEN(F17)-H17)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">LoadDeferredContent(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings parentSettings, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="str">
-        <f>RIGHT(D18,LEN(D18)-FIND("Line ",D18)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 866</v>
       </c>
       <c r="F18" t="str">
-        <f>LEFT(D18,LEN(D18)-LEN(E18))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.ResourceDictionary.CreateObject(System.Windows.Baml2006.KeyRecord key) </v>
       </c>
       <c r="G18" t="str">
-        <f>LEFT(F18,FIND("(",F18))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.ResourceDictionary.CreateObject(</v>
       </c>
       <c r="H18">
-        <f>FIND("@",SUBSTITUTE(G18,".","@",LEN(G18)-LEN(SUBSTITUTE(G18,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I18" t="str">
-        <f>RIGHT(F18,LEN(F18)-H18)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">CreateObject(System.Windows.Baml2006.KeyRecord key) </v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="str">
-        <f>RIGHT(D19,LEN(D19)-FIND("Line ",D19)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 708</v>
       </c>
       <c r="F19" t="str">
-        <f>LEFT(D19,LEN(D19)-LEN(E19))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.ResourceDictionary.OnGettingValue(object key, ref object value, out bool canCache) </v>
       </c>
       <c r="G19" t="str">
-        <f>LEFT(F19,FIND("(",F19))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.ResourceDictionary.OnGettingValue(</v>
       </c>
       <c r="H19">
-        <f>FIND("@",SUBSTITUTE(G19,".","@",LEN(G19)-LEN(SUBSTITUTE(G19,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I19" t="str">
-        <f>RIGHT(F19,LEN(F19)-H19)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">OnGettingValue(object key, ref object value, out bool canCache) </v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="str">
-        <f>RIGHT(D20,LEN(D20)-FIND("Line ",D20)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 680</v>
       </c>
       <c r="F20" t="str">
-        <f>LEFT(D20,LEN(D20)-LEN(E20))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.ResourceDictionary.OnGettingValuePrivate(object key, ref object value, out bool canCache) </v>
       </c>
       <c r="G20" t="str">
-        <f>LEFT(F20,FIND("(",F20))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.ResourceDictionary.OnGettingValuePrivate(</v>
       </c>
       <c r="H20">
-        <f>FIND("@",SUBSTITUTE(G20,".","@",LEN(G20)-LEN(SUBSTITUTE(G20,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I20" t="str">
-        <f>RIGHT(F20,LEN(F20)-H20)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">OnGettingValuePrivate(object key, ref object value, out bool canCache) </v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="E21" t="str">
-        <f>RIGHT(D21,LEN(D21)-FIND("Line ",D21)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 456</v>
       </c>
       <c r="F21" t="str">
-        <f>LEFT(D21,LEN(D21)-LEN(E21))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.ResourceDictionary.GetValueWithoutLock(object key, out bool canCache) </v>
       </c>
       <c r="G21" t="str">
-        <f>LEFT(F21,FIND("(",F21))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.ResourceDictionary.GetValueWithoutLock(</v>
       </c>
       <c r="H21">
-        <f>FIND("@",SUBSTITUTE(G21,".","@",LEN(G21)-LEN(SUBSTITUTE(G21,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I21" t="str">
-        <f>RIGHT(F21,LEN(F21)-H21)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">GetValueWithoutLock(object key, out bool canCache) </v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="str">
-        <f>RIGHT(D22,LEN(D22)-FIND("Line ",D22)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 446</v>
       </c>
       <c r="F22" t="str">
-        <f>LEFT(D22,LEN(D22)-LEN(E22))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.ResourceDictionary.GetValue(object key, out bool canCache) </v>
       </c>
       <c r="G22" t="str">
-        <f>LEFT(F22,FIND("(",F22))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.ResourceDictionary.GetValue(</v>
       </c>
       <c r="H22">
-        <f>FIND("@",SUBSTITUTE(G22,".","@",LEN(G22)-LEN(SUBSTITUTE(G22,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="I22" t="str">
-        <f>RIGHT(F22,LEN(F22)-H22)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">GetValue(object key, out bool canCache) </v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="str">
-        <f>RIGHT(D23,LEN(D23)-FIND("Line ",D23)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 164</v>
       </c>
       <c r="F23" t="str">
-        <f>LEFT(D23,LEN(D23)-LEN(E23))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.StaticResourceExtension.FindResourceInEnviroment(System.IServiceProvider serviceProvider, bool allowDeferredReference, bool mustReturnDeferredResourceReference) </v>
       </c>
       <c r="G23" t="str">
-        <f>LEFT(F23,FIND("(",F23))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.StaticResourceExtension.FindResourceInEnviroment(</v>
       </c>
       <c r="H23">
-        <f>FIND("@",SUBSTITUTE(G23,".","@",LEN(G23)-LEN(SUBSTITUTE(G23,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="I23" t="str">
-        <f>RIGHT(F23,LEN(F23)-H23)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">FindResourceInEnviroment(System.IServiceProvider serviceProvider, bool allowDeferredReference, bool mustReturnDeferredResourceReference) </v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
       <c r="E24" t="str">
-        <f>RIGHT(D24,LEN(D24)-FIND("Line ",D24)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 86</v>
       </c>
       <c r="F24" t="str">
-        <f>LEFT(D24,LEN(D24)-LEN(E24))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.StaticResourceExtension.TryProvideValueInternal(System.IServiceProvider serviceProvider, bool allowDeferredReference, bool mustReturnDeferredResourceReference) </v>
       </c>
       <c r="G24" t="str">
-        <f>LEFT(F24,FIND("(",F24))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.StaticResourceExtension.TryProvideValueInternal(</v>
       </c>
       <c r="H24">
-        <f>FIND("@",SUBSTITUTE(G24,".","@",LEN(G24)-LEN(SUBSTITUTE(G24,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="I24" t="str">
-        <f>RIGHT(F24,LEN(F24)-H24)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">TryProvideValueInternal(System.IServiceProvider serviceProvider, bool allowDeferredReference, bool mustReturnDeferredResourceReference) </v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
       <c r="E25" t="str">
-        <f>RIGHT(D25,LEN(D25)-FIND("Line ",D25)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 76</v>
       </c>
       <c r="F25" t="str">
-        <f>LEFT(D25,LEN(D25)-LEN(E25))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.StaticResourceExtension.ProvideValueInternal(System.IServiceProvider serviceProvider, bool allowDeferredReference) </v>
       </c>
       <c r="G25" t="str">
-        <f>LEFT(F25,FIND("(",F25))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.StaticResourceExtension.ProvideValueInternal(</v>
       </c>
       <c r="H25">
-        <f>FIND("@",SUBSTITUTE(G25,".","@",LEN(G25)-LEN(SUBSTITUTE(G25,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="I25" t="str">
-        <f>RIGHT(F25,LEN(F25)-H25)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">ProvideValueInternal(System.IServiceProvider serviceProvider, bool allowDeferredReference) </v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="D26" t="s">
         <v>364</v>
       </c>
       <c r="E26" t="str">
-        <f>RIGHT(D26,LEN(D26)-FIND("Line ",D26)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 71</v>
       </c>
       <c r="F26" t="str">
-        <f>LEFT(D26,LEN(D26)-LEN(E26))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.StaticResourceExtension.ProvideValue(System.IServiceProvider serviceProvider) </v>
       </c>
       <c r="G26" t="str">
-        <f>LEFT(F26,FIND("(",F26))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.StaticResourceExtension.ProvideValue(</v>
       </c>
       <c r="H26">
-        <f>FIND("@",SUBSTITUTE(G26,".","@",LEN(G26)-LEN(SUBSTITUTE(G26,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="I26" t="str">
-        <f>RIGHT(F26,LEN(F26)-H26)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">ProvideValue(System.IServiceProvider serviceProvider) </v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>18</v>
       </c>
       <c r="E27" t="str">
-        <f>RIGHT(D27,LEN(D27)-FIND("Line ",D27)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 416</v>
       </c>
       <c r="F27" t="str">
-        <f>LEFT(D27,LEN(D27)-LEN(E27))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CallProvideValue(System.Windows.Markup.MarkupExtension me, System.IServiceProvider serviceProvider) </v>
       </c>
       <c r="G27" t="str">
-        <f>LEFT(F27,FIND("(",F27))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CallProvideValue(</v>
       </c>
       <c r="H27">
-        <f>FIND("@",SUBSTITUTE(G27,".","@",LEN(G27)-LEN(SUBSTITUTE(G27,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>58</v>
       </c>
       <c r="I27" t="str">
-        <f>RIGHT(F27,LEN(F27)-H27)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">CallProvideValue(System.Windows.Markup.MarkupExtension me, System.IServiceProvider serviceProvider) </v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
       </c>
       <c r="E28" t="str">
-        <f>RIGHT(D28,LEN(D28)-FIND("Line ",D28)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 1173</v>
       </c>
       <c r="F28" t="str">
-        <f>LEFT(D28,LEN(D28)-LEN(E28))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_ProvideValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
       <c r="G28" t="str">
-        <f>LEFT(F28,FIND("(",F28))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_ProvideValue(</v>
       </c>
       <c r="H28">
-        <f>FIND("@",SUBSTITUTE(G28,".","@",LEN(G28)-LEN(SUBSTITUTE(G28,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I28" t="str">
-        <f>RIGHT(F28,LEN(F28)-H28)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Logic_ProvideValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="str">
-        <f>RIGHT(D29,LEN(D29)-FIND("Line ",D29)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 1135</v>
       </c>
       <c r="F29" t="str">
-        <f>LEFT(D29,LEN(D29)-LEN(E29))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_AssignProvidedValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
       <c r="G29" t="str">
-        <f>LEFT(F29,FIND("(",F29))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_AssignProvidedValue(</v>
       </c>
       <c r="H29">
-        <f>FIND("@",SUBSTITUTE(G29,".","@",LEN(G29)-LEN(SUBSTITUTE(G29,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I29" t="str">
-        <f>RIGHT(F29,LEN(F29)-H29)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">Logic_AssignProvidedValue(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="str">
-        <f>RIGHT(D30,LEN(D30)-FIND("Line ",D30)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 577</v>
       </c>
       <c r="F30" t="str">
-        <f>LEFT(D30,LEN(D30)-LEN(E30))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteEndMember() </v>
       </c>
       <c r="G30" t="str">
-        <f>LEFT(F30,FIND("(",F30))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteEndMember(</v>
       </c>
       <c r="H30">
-        <f>FIND("@",SUBSTITUTE(G30,".","@",LEN(G30)-LEN(SUBSTITUTE(G30,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I30" t="str">
-        <f>RIGHT(F30,LEN(F30)-H30)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">WriteEndMember() </v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>362</v>
       </c>
       <c r="E31" t="str">
-        <f>RIGHT(D31,LEN(D31)-FIND("Line ",D31)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 72</v>
       </c>
       <c r="F31" t="str">
-        <f>LEFT(D31,LEN(D31)-LEN(E31))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
       <c r="G31" t="str">
-        <f>LEFT(F31,FIND("(",F31))</f>
+        <f t="shared" si="2"/>
         <v>System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(</v>
       </c>
       <c r="H31">
-        <f>FIND("@",SUBSTITUTE(G31,".","@",LEN(G31)-LEN(SUBSTITUTE(G31,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="I31" t="str">
-        <f>RIGHT(F31,LEN(F31)-H31)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
       <c r="E32" t="str">
-        <f>RIGHT(D32,LEN(D32)-FIND("Line ",D32)+1)</f>
+        <f t="shared" si="0"/>
         <v>Line 229</v>
       </c>
       <c r="F32" t="str">
-        <f>LEFT(D32,LEN(D32)-LEN(E32))</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
       <c r="G32" t="str">
-        <f>LEFT(F32,FIND("(",F32))</f>
+        <f t="shared" si="2"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(</v>
       </c>
       <c r="H32">
-        <f>FIND("@",SUBSTITUTE(G32,".","@",LEN(G32)-LEN(SUBSTITUTE(G32,".",""))))</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="I32" t="str">
-        <f>RIGHT(F32,LEN(F32)-H32)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="str">
-        <f>RIGHT(D33,LEN(D33)-FIND("Line ",D33)+1)</f>
+        <f t="shared" ref="E33:E64" si="7">RIGHT(D33,LEN(D33)-FIND("Line ",D33)+1)</f>
         <v>Line 105</v>
       </c>
       <c r="F33" t="str">
-        <f>LEFT(D33,LEN(D33)-LEN(E33))</f>
+        <f t="shared" ref="F33:F64" si="8">LEFT(D33,LEN(D33)-LEN(E33))</f>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
       <c r="G33" t="str">
-        <f>LEFT(F33,FIND("(",F33))</f>
+        <f t="shared" ref="G33:G64" si="9">LEFT(F33,FIND("(",F33))</f>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(</v>
       </c>
       <c r="H33">
-        <f>FIND("@",SUBSTITUTE(G33,".","@",LEN(G33)-LEN(SUBSTITUTE(G33,".",""))))</f>
+        <f t="shared" ref="H33:H64" si="10">FIND("@",SUBSTITUTE(G33,".","@",LEN(G33)-LEN(SUBSTITUTE(G33,".",""))))</f>
         <v>62</v>
       </c>
       <c r="I33" t="str">
-        <f>RIGHT(F33,LEN(F33)-H33)</f>
+        <f t="shared" ref="I33:I64" si="11">RIGHT(F33,LEN(F33)-H33)</f>
         <v xml:space="preserve">Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
       </c>
       <c r="E34" t="str">
-        <f>RIGHT(D34,LEN(D34)-FIND("Line ",D34)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 42</v>
       </c>
       <c r="F34" t="str">
-        <f>LEFT(D34,LEN(D34)-LEN(E34))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadBaml(System.Xaml.XamlReader xamlReader, bool skipJournaledProperties, object rootObject, System.Xaml.Permissions.XamlAccessLevel accessLevel, System.Uri baseUri) </v>
       </c>
       <c r="G34" t="str">
-        <f>LEFT(F34,FIND("(",F34))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadBaml(</v>
       </c>
       <c r="H34">
-        <f>FIND("@",SUBSTITUTE(G34,".","@",LEN(G34)-LEN(SUBSTITUTE(G34,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="I34" t="str">
-        <f>RIGHT(F34,LEN(F34)-H34)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadBaml(System.Xaml.XamlReader xamlReader, bool skipJournaledProperties, object rootObject, System.Xaml.Permissions.XamlAccessLevel accessLevel, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>365</v>
       </c>
       <c r="E35" t="str">
-        <f>RIGHT(D35,LEN(D35)-FIND("Line ",D35)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 616</v>
       </c>
       <c r="F35" t="str">
-        <f>LEFT(D35,LEN(D35)-LEN(E35))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.XamlReader.LoadBaml(System.IO.Stream stream, System.Windows.Markup.ParserContext parserContext, object parent, bool closeStream) </v>
       </c>
       <c r="G35" t="str">
-        <f>LEFT(F35,FIND("(",F35))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.XamlReader.LoadBaml(</v>
       </c>
       <c r="H35">
-        <f>FIND("@",SUBSTITUTE(G35,".","@",LEN(G35)-LEN(SUBSTITUTE(G35,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>59</v>
       </c>
       <c r="I35" t="str">
-        <f>RIGHT(F35,LEN(F35)-H35)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadBaml(System.IO.Stream stream, System.Windows.Markup.ParserContext parserContext, object parent, bool closeStream) </v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="D36" t="s">
         <v>366</v>
       </c>
       <c r="E36" t="str">
-        <f>RIGHT(D36,LEN(D36)-FIND("Line ",D36)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 726</v>
       </c>
       <c r="F36" t="str">
-        <f>LEFT(D36,LEN(D36)-LEN(E36))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Application.LoadComponent(object component, System.Uri resourceLocator) </v>
       </c>
       <c r="G36" t="str">
-        <f>LEFT(F36,FIND("(",F36))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Application.LoadComponent(</v>
       </c>
       <c r="H36">
-        <f>FIND("@",SUBSTITUTE(G36,".","@",LEN(G36)-LEN(SUBSTITUTE(G36,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
       <c r="I36" t="str">
-        <f>RIGHT(F36,LEN(F36)-H36)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadComponent(object component, System.Uri resourceLocator) </v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
       </c>
       <c r="E37" t="str">
-        <f>RIGHT(D37,LEN(D37)-FIND("Line ",D37)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 1</v>
       </c>
       <c r="F37" t="str">
-        <f>LEFT(D37,LEN(D37)-LEN(E37))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">Spec.exe!Spec.Plain.MTCMinimal.InitializeComponent() </v>
       </c>
       <c r="G37" t="str">
-        <f>LEFT(F37,FIND("(",F37))</f>
+        <f t="shared" si="9"/>
         <v>Spec.exe!Spec.Plain.MTCMinimal.InitializeComponent(</v>
       </c>
       <c r="H37">
-        <f>FIND("@",SUBSTITUTE(G37,".","@",LEN(G37)-LEN(SUBSTITUTE(G37,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="I37" t="str">
-        <f>RIGHT(F37,LEN(F37)-H37)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">InitializeComponent() </v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="D38" t="s">
         <v>357</v>
       </c>
       <c r="E38" t="str">
-        <f>RIGHT(D38,LEN(D38)-FIND("Line ",D38)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 19</v>
       </c>
       <c r="F38" t="str">
-        <f>LEFT(D38,LEN(D38)-LEN(E38))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">Spec.exe!Spec.Plain.MTCMinimal.MTCMinimal() </v>
       </c>
       <c r="G38" t="str">
-        <f>LEFT(F38,FIND("(",F38))</f>
+        <f t="shared" si="9"/>
         <v>Spec.exe!Spec.Plain.MTCMinimal.MTCMinimal(</v>
       </c>
       <c r="H38">
-        <f>FIND("@",SUBSTITUTE(G38,".","@",LEN(G38)-LEN(SUBSTITUTE(G38,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="I38" t="str">
-        <f>RIGHT(F38,LEN(F38)-H38)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">MTCMinimal() </v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="e">
-        <f>RIGHT(D39,LEN(D39)-FIND("Line ",D39)+1)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="F39" t="e">
-        <f>LEFT(D39,LEN(D39)-LEN(E39))</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G39" t="e">
-        <f>LEFT(F39,FIND("(",F39))</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="H39" t="e">
-        <f>FIND("@",SUBSTITUTE(G39,".","@",LEN(G39)-LEN(SUBSTITUTE(G39,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="I39" t="e">
-        <f>RIGHT(F39,LEN(F39)-H39)</f>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="D40" t="s">
         <v>60</v>
       </c>
       <c r="E40" t="e">
-        <f>RIGHT(D40,LEN(D40)-FIND("Line ",D40)+1)</f>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="F40" t="e">
-        <f>LEFT(D40,LEN(D40)-LEN(E40))</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G40" t="e">
-        <f>LEFT(F40,FIND("(",F40))</f>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="H40" t="e">
-        <f>FIND("@",SUBSTITUTE(G40,".","@",LEN(G40)-LEN(SUBSTITUTE(G40,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
       <c r="I40" t="e">
-        <f>RIGHT(F40,LEN(F40)-H40)</f>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="D41" t="s">
         <v>367</v>
       </c>
       <c r="E41" t="str">
-        <f>RIGHT(D41,LEN(D41)-FIND("Line ",D41)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 2227</v>
       </c>
       <c r="F41" t="str">
-        <f>LEFT(D41,LEN(D41)-LEN(E41))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">mscorlib.dll!System.RuntimeType.CreateInstanceSlow(bool publicOnly, bool skipCheckThis, bool fillCache, ref System.Threading.StackCrawlMark stackMark) </v>
       </c>
       <c r="G41" t="str">
-        <f>LEFT(F41,FIND("(",F41))</f>
+        <f t="shared" si="9"/>
         <v>mscorlib.dll!System.RuntimeType.CreateInstanceSlow(</v>
       </c>
       <c r="H41">
-        <f>FIND("@",SUBSTITUTE(G41,".","@",LEN(G41)-LEN(SUBSTITUTE(G41,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="I41" t="str">
-        <f>RIGHT(F41,LEN(F41)-H41)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstanceSlow(bool publicOnly, bool skipCheckThis, bool fillCache, ref System.Threading.StackCrawlMark stackMark) </v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="D42" t="s">
         <v>368</v>
       </c>
       <c r="E42" t="str">
-        <f>RIGHT(D42,LEN(D42)-FIND("Line ",D42)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 311</v>
       </c>
       <c r="F42" t="str">
-        <f>LEFT(D42,LEN(D42)-LEN(E42))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">mscorlib.dll!System.Activator.CreateInstance(System.Type type, bool nonPublic) </v>
       </c>
       <c r="G42" t="str">
-        <f>LEFT(F42,FIND("(",F42))</f>
+        <f t="shared" si="9"/>
         <v>mscorlib.dll!System.Activator.CreateInstance(</v>
       </c>
       <c r="H42">
-        <f>FIND("@",SUBSTITUTE(G42,".","@",LEN(G42)-LEN(SUBSTITUTE(G42,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="I42" t="str">
-        <f>RIGHT(F42,LEN(F42)-H42)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(System.Type type, bool nonPublic) </v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="D43" t="s">
         <v>369</v>
       </c>
       <c r="E43" t="str">
-        <f>RIGHT(D43,LEN(D43)-FIND("Line ",D43)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 2182</v>
       </c>
       <c r="F43" t="str">
-        <f>LEFT(D43,LEN(D43)-LEN(E43))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">mscorlib.dll!System.RuntimeType.CreateInstanceImpl(System.Reflection.BindingFlags bindingAttr, System.Reflection.Binder binder, object[] args, System.Globalization.CultureInfo culture, object[] activationAttributes, ref System.Threading.StackCrawlMark stackMark) </v>
       </c>
       <c r="G43" t="str">
-        <f>LEFT(F43,FIND("(",F43))</f>
+        <f t="shared" si="9"/>
         <v>mscorlib.dll!System.RuntimeType.CreateInstanceImpl(</v>
       </c>
       <c r="H43">
-        <f>FIND("@",SUBSTITUTE(G43,".","@",LEN(G43)-LEN(SUBSTITUTE(G43,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="I43" t="str">
-        <f>RIGHT(F43,LEN(F43)-H43)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstanceImpl(System.Reflection.BindingFlags bindingAttr, System.Reflection.Binder binder, object[] args, System.Globalization.CultureInfo culture, object[] activationAttributes, ref System.Threading.StackCrawlMark stackMark) </v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="D44" t="s">
         <v>370</v>
       </c>
       <c r="E44" t="str">
-        <f>RIGHT(D44,LEN(D44)-FIND("Line ",D44)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 121</v>
       </c>
       <c r="F44" t="str">
-        <f>LEFT(D44,LEN(D44)-LEN(E44))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">mscorlib.dll!System.Activator.CreateInstance(System.Type type, System.Reflection.BindingFlags bindingAttr, System.Reflection.Binder binder, object[] args, System.Globalization.CultureInfo culture, object[] activationAttributes) </v>
       </c>
       <c r="G44" t="str">
-        <f>LEFT(F44,FIND("(",F44))</f>
+        <f t="shared" si="9"/>
         <v>mscorlib.dll!System.Activator.CreateInstance(</v>
       </c>
       <c r="H44">
-        <f>FIND("@",SUBSTITUTE(G44,".","@",LEN(G44)-LEN(SUBSTITUTE(G44,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="I44" t="str">
-        <f>RIGHT(F44,LEN(F44)-H44)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(System.Type type, System.Reflection.BindingFlags bindingAttr, System.Reflection.Binder binder, object[] args, System.Globalization.CultureInfo culture, object[] activationAttributes) </v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="D45" t="s">
         <v>371</v>
       </c>
       <c r="E45" t="str">
-        <f>RIGHT(D45,LEN(D45)-FIND("Line ",D45)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 152</v>
       </c>
       <c r="F45" t="str">
-        <f>LEFT(D45,LEN(D45)-LEN(E45))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">mscorlib.dll!System.Activator.CreateInstance(System.Type type, object[] args) </v>
       </c>
       <c r="G45" t="str">
-        <f>LEFT(F45,FIND("(",F45))</f>
+        <f t="shared" si="9"/>
         <v>mscorlib.dll!System.Activator.CreateInstance(</v>
       </c>
       <c r="H45">
-        <f>FIND("@",SUBSTITUTE(G45,".","@",LEN(G45)-LEN(SUBSTITUTE(G45,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="I45" t="str">
-        <f>RIGHT(F45,LEN(F45)-H45)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(System.Type type, object[] args) </v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="D46" t="s">
         <v>30</v>
       </c>
       <c r="E46" t="str">
-        <f>RIGHT(D46,LEN(D46)-FIND("Line ",D46)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 192</v>
       </c>
       <c r="F46" t="str">
-        <f>LEFT(D46,LEN(D46)-LEN(E46))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.CreateInstanceCritical(System.Type type, object[] arguments) </v>
       </c>
       <c r="G46" t="str">
-        <f>LEFT(F46,FIND("(",F46))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.CreateInstanceCritical(</v>
       </c>
       <c r="H46">
-        <f>FIND("@",SUBSTITUTE(G46,".","@",LEN(G46)-LEN(SUBSTITUTE(G46,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>57</v>
       </c>
       <c r="I46" t="str">
-        <f>RIGHT(F46,LEN(F46)-H46)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstanceCritical(System.Type type, object[] arguments) </v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="D47" t="s">
         <v>372</v>
       </c>
       <c r="E47" t="str">
-        <f>RIGHT(D47,LEN(D47)-FIND("Line ",D47)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 186</v>
       </c>
       <c r="F47" t="str">
-        <f>LEFT(D47,LEN(D47)-LEN(E47))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.CreateInstance(System.Type type, object[] arguments) </v>
       </c>
       <c r="G47" t="str">
-        <f>LEFT(F47,FIND("(",F47))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.Schema.SafeReflectionInvoker.CreateInstance(</v>
       </c>
       <c r="H47">
-        <f>FIND("@",SUBSTITUTE(G47,".","@",LEN(G47)-LEN(SUBSTITUTE(G47,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>57</v>
       </c>
       <c r="I47" t="str">
-        <f>RIGHT(F47,LEN(F47)-H47)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(System.Type type, object[] arguments) </v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="D48" t="s">
         <v>31</v>
       </c>
       <c r="E48" t="str">
-        <f>RIGHT(D48,LEN(D48)-FIND("Line ",D48)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 186</v>
       </c>
       <c r="F48" t="str">
-        <f>LEFT(D48,LEN(D48)-LEN(E48))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.Schema.XamlTypeInvoker.CreateInstance(object[] arguments) </v>
       </c>
       <c r="G48" t="str">
-        <f>LEFT(F48,FIND("(",F48))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.Schema.XamlTypeInvoker.CreateInstance(</v>
       </c>
       <c r="H48">
-        <f>FIND("@",SUBSTITUTE(G48,".","@",LEN(G48)-LEN(SUBSTITUTE(G48,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>51</v>
       </c>
       <c r="I48" t="str">
-        <f>RIGHT(F48,LEN(F48)-H48)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(object[] arguments) </v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>49</v>
       </c>
       <c r="D49" t="s">
         <v>373</v>
       </c>
       <c r="E49" t="str">
-        <f>RIGHT(D49,LEN(D49)-FIND("Line ",D49)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 65</v>
       </c>
       <c r="F49" t="str">
-        <f>LEFT(D49,LEN(D49)-LEN(E49))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CreateInstanceWithCtor(System.Xaml.XamlType xamlType, object[] args) </v>
       </c>
       <c r="G49" t="str">
-        <f>LEFT(F49,FIND("(",F49))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CreateInstanceWithCtor(</v>
       </c>
       <c r="H49">
-        <f>FIND("@",SUBSTITUTE(G49,".","@",LEN(G49)-LEN(SUBSTITUTE(G49,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>58</v>
       </c>
       <c r="I49" t="str">
-        <f>RIGHT(F49,LEN(F49)-H49)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstanceWithCtor(System.Xaml.XamlType xamlType, object[] args) </v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
       </c>
       <c r="E50" t="str">
-        <f>RIGHT(D50,LEN(D50)-FIND("Line ",D50)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 48</v>
       </c>
       <c r="F50" t="str">
-        <f>LEFT(D50,LEN(D50)-LEN(E50))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CreateInstance(System.Xaml.XamlType xamlType, object[] args) </v>
       </c>
       <c r="G50" t="str">
-        <f>LEFT(F50,FIND("(",F50))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!MS.Internal.Xaml.Runtime.ClrObjectRuntime.CreateInstance(</v>
       </c>
       <c r="H50">
-        <f>FIND("@",SUBSTITUTE(G50,".","@",LEN(G50)-LEN(SUBSTITUTE(G50,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>58</v>
       </c>
       <c r="I50" t="str">
-        <f>RIGHT(F50,LEN(F50)-H50)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">CreateInstance(System.Xaml.XamlType xamlType, object[] args) </v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>51</v>
       </c>
       <c r="D51" t="s">
         <v>33</v>
       </c>
       <c r="E51" t="str">
-        <f>RIGHT(D51,LEN(D51)-FIND("Line ",D51)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 804</v>
       </c>
       <c r="F51" t="str">
-        <f>LEFT(D51,LEN(D51)-LEN(E51))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_CreateAndAssignToParentStart(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
       <c r="G51" t="str">
-        <f>LEFT(F51,FIND("(",F51))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.Logic_CreateAndAssignToParentStart(</v>
       </c>
       <c r="H51">
-        <f>FIND("@",SUBSTITUTE(G51,".","@",LEN(G51)-LEN(SUBSTITUTE(G51,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="I51" t="str">
-        <f>RIGHT(F51,LEN(F51)-H51)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Logic_CreateAndAssignToParentStart(MS.Internal.Xaml.Context.ObjectWriterContext ctx) </v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>52</v>
       </c>
       <c r="C52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="D52" t="s">
         <v>34</v>
       </c>
       <c r="E52" t="str">
-        <f>RIGHT(D52,LEN(D52)-FIND("Line ",D52)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 498</v>
       </c>
       <c r="F52" t="str">
-        <f>LEFT(D52,LEN(D52)-LEN(E52))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteStartMember(System.Xaml.XamlMember property) </v>
       </c>
       <c r="G52" t="str">
-        <f>LEFT(F52,FIND("(",F52))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.XamlObjectWriter.WriteStartMember(</v>
       </c>
       <c r="H52">
-        <f>FIND("@",SUBSTITUTE(G52,".","@",LEN(G52)-LEN(SUBSTITUTE(G52,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>45</v>
       </c>
       <c r="I52" t="str">
-        <f>RIGHT(F52,LEN(F52)-H52)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">WriteStartMember(System.Xaml.XamlMember property) </v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
       <c r="C53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="D53" t="s">
         <v>374</v>
       </c>
       <c r="E53" t="str">
-        <f>RIGHT(D53,LEN(D53)-FIND("Line ",D53)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 69</v>
       </c>
       <c r="F53" t="str">
-        <f>LEFT(D53,LEN(D53)-LEN(E53))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
       <c r="G53" t="str">
-        <f>LEFT(F53,FIND("(",F53))</f>
+        <f t="shared" si="9"/>
         <v>System.Xaml.dll!System.Xaml.XamlWriter.WriteNode(</v>
       </c>
       <c r="H53">
-        <f>FIND("@",SUBSTITUTE(G53,".","@",LEN(G53)-LEN(SUBSTITUTE(G53,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>39</v>
       </c>
       <c r="I53" t="str">
-        <f>RIGHT(F53,LEN(F53)-H53)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">WriteNode(System.Xaml.XamlReader reader) </v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>54</v>
       </c>
       <c r="C54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="D54" t="s">
         <v>35</v>
       </c>
       <c r="E54" t="str">
-        <f>RIGHT(D54,LEN(D54)-FIND("Line ",D54)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 163</v>
       </c>
       <c r="F54" t="str">
-        <f>LEFT(D54,LEN(D54)-LEN(E54))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
       <c r="G54" t="str">
-        <f>LEFT(F54,FIND("(",F54))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.TransformNodes(</v>
       </c>
       <c r="H54">
-        <f>FIND("@",SUBSTITUTE(G54,".","@",LEN(G54)-LEN(SUBSTITUTE(G54,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="I54" t="str">
-        <f>RIGHT(F54,LEN(F54)-H54)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">TransformNodes(System.Xaml.XamlReader xamlReader, System.Xaml.XamlObjectWriter xamlWriter, bool onlyLoadOneNode, bool skipJournaledProperties, bool shouldPassLineNumberInfo, System.Xaml.IXamlLineInfo xamlLineInfo, System.Xaml.IXamlLineInfoConsumer xamlLineInfoConsumer, MS.Internal.Xaml.Context.XamlContextStack&lt;System.Windows.Markup.WpfXamlFrame&gt; stack, System.Windows.Markup.IStyleConnector styleConnector) </v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="C55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>55</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
       </c>
       <c r="E55" t="str">
-        <f>RIGHT(D55,LEN(D55)-FIND("Line ",D55)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 105</v>
       </c>
       <c r="F55" t="str">
-        <f>LEFT(D55,LEN(D55)-LEN(E55))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
       <c r="G55" t="str">
-        <f>LEFT(F55,FIND("(",F55))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.Load(</v>
       </c>
       <c r="H55">
-        <f>FIND("@",SUBSTITUTE(G55,".","@",LEN(G55)-LEN(SUBSTITUTE(G55,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="I55" t="str">
-        <f>RIGHT(F55,LEN(F55)-H55)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Load(System.Xaml.XamlReader xamlReader, System.Xaml.IXamlObjectWriterFactory writerFactory, bool skipJournaledProperties, object rootObject, System.Xaml.XamlObjectWriterSettings settings, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="C56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
       </c>
       <c r="E56" t="str">
-        <f>RIGHT(D56,LEN(D56)-FIND("Line ",D56)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 42</v>
       </c>
       <c r="F56" t="str">
-        <f>LEFT(D56,LEN(D56)-LEN(E56))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadBaml(System.Xaml.XamlReader xamlReader, bool skipJournaledProperties, object rootObject, System.Xaml.Permissions.XamlAccessLevel accessLevel, System.Uri baseUri) </v>
       </c>
       <c r="G56" t="str">
-        <f>LEFT(F56,FIND("(",F56))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.WpfXamlLoader.LoadBaml(</v>
       </c>
       <c r="H56">
-        <f>FIND("@",SUBSTITUTE(G56,".","@",LEN(G56)-LEN(SUBSTITUTE(G56,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="I56" t="str">
-        <f>RIGHT(F56,LEN(F56)-H56)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadBaml(System.Xaml.XamlReader xamlReader, bool skipJournaledProperties, object rootObject, System.Xaml.Permissions.XamlAccessLevel accessLevel, System.Uri baseUri) </v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
       <c r="C57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>57</v>
       </c>
       <c r="D57" t="s">
         <v>365</v>
       </c>
       <c r="E57" t="str">
-        <f>RIGHT(D57,LEN(D57)-FIND("Line ",D57)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 616</v>
       </c>
       <c r="F57" t="str">
-        <f>LEFT(D57,LEN(D57)-LEN(E57))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Markup.XamlReader.LoadBaml(System.IO.Stream stream, System.Windows.Markup.ParserContext parserContext, object parent, bool closeStream) </v>
       </c>
       <c r="G57" t="str">
-        <f>LEFT(F57,FIND("(",F57))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Markup.XamlReader.LoadBaml(</v>
       </c>
       <c r="H57">
-        <f>FIND("@",SUBSTITUTE(G57,".","@",LEN(G57)-LEN(SUBSTITUTE(G57,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>59</v>
       </c>
       <c r="I57" t="str">
-        <f>RIGHT(F57,LEN(F57)-H57)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadBaml(System.IO.Stream stream, System.Windows.Markup.ParserContext parserContext, object parent, bool closeStream) </v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>58</v>
       </c>
       <c r="C58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>58</v>
       </c>
       <c r="D58" t="s">
         <v>36</v>
       </c>
       <c r="E58" t="str">
-        <f>RIGHT(D58,LEN(D58)-FIND("Line ",D58)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 774</v>
       </c>
       <c r="F58" t="str">
-        <f>LEFT(D58,LEN(D58)-LEN(E58))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Application.LoadBamlStreamWithSyncInfo(System.IO.Stream stream, System.Windows.Markup.ParserContext pc) </v>
       </c>
       <c r="G58" t="str">
-        <f>LEFT(F58,FIND("(",F58))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Application.LoadBamlStreamWithSyncInfo(</v>
       </c>
       <c r="H58">
-        <f>FIND("@",SUBSTITUTE(G58,".","@",LEN(G58)-LEN(SUBSTITUTE(G58,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
       <c r="I58" t="str">
-        <f>RIGHT(F58,LEN(F58)-H58)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadBamlStreamWithSyncInfo(System.IO.Stream stream, System.Windows.Markup.ParserContext pc) </v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>59</v>
       </c>
       <c r="C59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>59</v>
       </c>
       <c r="D59" t="s">
         <v>375</v>
       </c>
       <c r="E59" t="str">
-        <f>RIGHT(D59,LEN(D59)-FIND("Line ",D59)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 763</v>
       </c>
       <c r="F59" t="str">
-        <f>LEFT(D59,LEN(D59)-LEN(E59))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Application.LoadComponent(System.Uri resourceLocator, bool bSkipJournaledProperties) </v>
       </c>
       <c r="G59" t="str">
-        <f>LEFT(F59,FIND("(",F59))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Application.LoadComponent(</v>
       </c>
       <c r="H59">
-        <f>FIND("@",SUBSTITUTE(G59,".","@",LEN(G59)-LEN(SUBSTITUTE(G59,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
       <c r="I59" t="str">
-        <f>RIGHT(F59,LEN(F59)-H59)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadComponent(System.Uri resourceLocator, bool bSkipJournaledProperties) </v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="C60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="D60" t="s">
         <v>376</v>
       </c>
       <c r="E60" t="str">
-        <f>RIGHT(D60,LEN(D60)-FIND("Line ",D60)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 745</v>
       </c>
       <c r="F60" t="str">
-        <f>LEFT(D60,LEN(D60)-LEN(E60))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Application.LoadComponent(System.Uri resourceLocator) </v>
       </c>
       <c r="G60" t="str">
-        <f>LEFT(F60,FIND("(",F60))</f>
+        <f t="shared" si="9"/>
         <v>PresentationFramework.dll!System.Windows.Application.LoadComponent(</v>
       </c>
       <c r="H60">
-        <f>FIND("@",SUBSTITUTE(G60,".","@",LEN(G60)-LEN(SUBSTITUTE(G60,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>53</v>
       </c>
       <c r="I60" t="str">
-        <f>RIGHT(F60,LEN(F60)-H60)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">LoadComponent(System.Uri resourceLocator) </v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>61</v>
       </c>
       <c r="C61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>61</v>
       </c>
       <c r="D61" t="s">
         <v>37</v>
       </c>
       <c r="E61" t="str">
-        <f>RIGHT(D61,LEN(D61)-FIND("Line ",D61)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 22</v>
       </c>
       <c r="F61" t="str">
-        <f>LEFT(D61,LEN(D61)-LEN(E61))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">Spec.exe!Spec.MainWindow.Panel_OnClick(object sender, System.Windows.RoutedEventArgs e) </v>
       </c>
       <c r="G61" t="str">
-        <f>LEFT(F61,FIND("(",F61))</f>
+        <f t="shared" si="9"/>
         <v>Spec.exe!Spec.MainWindow.Panel_OnClick(</v>
       </c>
       <c r="H61">
-        <f>FIND("@",SUBSTITUTE(G61,".","@",LEN(G61)-LEN(SUBSTITUTE(G61,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
       <c r="I61" t="str">
-        <f>RIGHT(F61,LEN(F61)-H61)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Panel_OnClick(object sender, System.Windows.RoutedEventArgs e) </v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>62</v>
       </c>
       <c r="C62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>62</v>
       </c>
       <c r="D62" t="s">
         <v>44</v>
       </c>
       <c r="E62" t="str">
-        <f>RIGHT(D62,LEN(D62)-FIND("Line ",D62)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 66</v>
       </c>
       <c r="F62" t="str">
-        <f>LEFT(D62,LEN(D62)-LEN(E62))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
       <c r="G62" t="str">
-        <f>LEFT(F62,FIND("(",F62))</f>
+        <f t="shared" si="9"/>
         <v>PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(</v>
       </c>
       <c r="H62">
-        <f>FIND("@",SUBSTITUTE(G62,".","@",LEN(G62)-LEN(SUBSTITUTE(G62,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>59</v>
       </c>
       <c r="I62" t="str">
-        <f>RIGHT(F62,LEN(F62)-H62)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>63</v>
       </c>
       <c r="C63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="D63" t="s">
         <v>38</v>
       </c>
       <c r="E63" t="str">
-        <f>RIGHT(D63,LEN(D63)-FIND("Line ",D63)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 103</v>
       </c>
       <c r="F63" t="str">
-        <f>LEFT(D63,LEN(D63)-LEN(E63))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
       <c r="G63" t="str">
-        <f>LEFT(F63,FIND("(",F63))</f>
+        <f t="shared" si="9"/>
         <v>PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(</v>
       </c>
       <c r="H63">
-        <f>FIND("@",SUBSTITUTE(G63,".","@",LEN(G63)-LEN(SUBSTITUTE(G63,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>47</v>
       </c>
       <c r="I63" t="str">
-        <f>RIGHT(F63,LEN(F63)-H63)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="C64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="D64" t="s">
         <v>39</v>
       </c>
       <c r="E64" t="str">
-        <f>RIGHT(D64,LEN(D64)-FIND("Line ",D64)+1)</f>
+        <f t="shared" si="7"/>
         <v>Line 6098</v>
       </c>
       <c r="F64" t="str">
-        <f>LEFT(D64,LEN(D64)-LEN(E64))</f>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.UIElement.RaiseEventImpl(System.Windows.DependencyObject sender, System.Windows.RoutedEventArgs args) </v>
       </c>
       <c r="G64" t="str">
-        <f>LEFT(F64,FIND("(",F64))</f>
+        <f t="shared" si="9"/>
         <v>PresentationCore.dll!System.Windows.UIElement.RaiseEventImpl(</v>
       </c>
       <c r="H64">
-        <f>FIND("@",SUBSTITUTE(G64,".","@",LEN(G64)-LEN(SUBSTITUTE(G64,".",""))))</f>
+        <f t="shared" si="10"/>
         <v>46</v>
       </c>
       <c r="I64" t="str">
-        <f>RIGHT(F64,LEN(F64)-H64)</f>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">RaiseEventImpl(System.Windows.DependencyObject sender, System.Windows.RoutedEventArgs args) </v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>65</v>
       </c>
       <c r="C65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
       <c r="D65" t="s">
         <v>377</v>
       </c>
       <c r="E65" t="str">
-        <f>RIGHT(D65,LEN(D65)-FIND("Line ",D65)+1)</f>
+        <f t="shared" ref="E65:E96" si="12">RIGHT(D65,LEN(D65)-FIND("Line ",D65)+1)</f>
         <v>Line 2687</v>
       </c>
       <c r="F65" t="str">
-        <f>LEFT(D65,LEN(D65)-LEN(E65))</f>
+        <f t="shared" ref="F65:F96" si="13">LEFT(D65,LEN(D65)-LEN(E65))</f>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.UIElement.RaiseEvent(System.Windows.RoutedEventArgs e) </v>
       </c>
       <c r="G65" t="str">
-        <f>LEFT(F65,FIND("(",F65))</f>
+        <f t="shared" ref="G65:G96" si="14">LEFT(F65,FIND("(",F65))</f>
         <v>PresentationCore.dll!System.Windows.UIElement.RaiseEvent(</v>
       </c>
       <c r="H65">
-        <f>FIND("@",SUBSTITUTE(G65,".","@",LEN(G65)-LEN(SUBSTITUTE(G65,".",""))))</f>
+        <f t="shared" ref="H65:H96" si="15">FIND("@",SUBSTITUTE(G65,".","@",LEN(G65)-LEN(SUBSTITUTE(G65,".",""))))</f>
         <v>46</v>
       </c>
       <c r="I65" t="str">
-        <f>RIGHT(F65,LEN(F65)-H65)</f>
+        <f t="shared" ref="I65:I96" si="16">RIGHT(F65,LEN(F65)-H65)</f>
         <v xml:space="preserve">RaiseEvent(System.Windows.RoutedEventArgs e) </v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>66</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C79" si="2">$A66-B66</f>
+        <f t="shared" ref="C66:C79" si="17">$A66-B66</f>
         <v>66</v>
       </c>
       <c r="D66" t="s">
         <v>40</v>
       </c>
       <c r="E66" t="str">
-        <f>RIGHT(D66,LEN(D66)-FIND("Line ",D66)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 206</v>
       </c>
       <c r="F66" t="str">
-        <f>LEFT(D66,LEN(D66)-LEN(E66))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Controls.Primitives.ButtonBase.OnClick() </v>
       </c>
       <c r="G66" t="str">
-        <f>LEFT(F66,FIND("(",F66))</f>
+        <f t="shared" si="14"/>
         <v>PresentationFramework.dll!System.Windows.Controls.Primitives.ButtonBase.OnClick(</v>
       </c>
       <c r="H66">
-        <f>FIND("@",SUBSTITUTE(G66,".","@",LEN(G66)-LEN(SUBSTITUTE(G66,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>72</v>
       </c>
       <c r="I66" t="str">
-        <f>RIGHT(F66,LEN(F66)-H66)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">OnClick() </v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" ref="A67:A79" si="3">C66+1</f>
+        <f t="shared" ref="A67:A79" si="18">C66+1</f>
         <v>67</v>
       </c>
       <c r="C67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>67</v>
       </c>
       <c r="D67" t="s">
         <v>41</v>
       </c>
       <c r="E67" t="str">
-        <f>RIGHT(D67,LEN(D67)-FIND("Line ",D67)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 185</v>
       </c>
       <c r="F67" t="str">
-        <f>LEFT(D67,LEN(D67)-LEN(E67))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Controls.Button.OnClick() </v>
       </c>
       <c r="G67" t="str">
-        <f>LEFT(F67,FIND("(",F67))</f>
+        <f t="shared" si="14"/>
         <v>PresentationFramework.dll!System.Windows.Controls.Button.OnClick(</v>
       </c>
       <c r="H67">
-        <f>FIND("@",SUBSTITUTE(G67,".","@",LEN(G67)-LEN(SUBSTITUTE(G67,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>57</v>
       </c>
       <c r="I67" t="str">
-        <f>RIGHT(F67,LEN(F67)-H67)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">OnClick() </v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>68</v>
       </c>
       <c r="C68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>68</v>
       </c>
       <c r="D68" t="s">
         <v>42</v>
       </c>
       <c r="E68" t="str">
-        <f>RIGHT(D68,LEN(D68)-FIND("Line ",D68)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 376</v>
       </c>
       <c r="F68" t="str">
-        <f>LEFT(D68,LEN(D68)-LEN(E68))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationFramework.dll!System.Windows.Controls.Primitives.ButtonBase.OnMouseLeftButtonUp(System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
       <c r="G68" t="str">
-        <f>LEFT(F68,FIND("(",F68))</f>
+        <f t="shared" si="14"/>
         <v>PresentationFramework.dll!System.Windows.Controls.Primitives.ButtonBase.OnMouseLeftButtonUp(</v>
       </c>
       <c r="H68">
-        <f>FIND("@",SUBSTITUTE(G68,".","@",LEN(G68)-LEN(SUBSTITUTE(G68,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>72</v>
       </c>
       <c r="I68" t="str">
-        <f>RIGHT(F68,LEN(F68)-H68)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">OnMouseLeftButtonUp(System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>69</v>
       </c>
       <c r="C69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>69</v>
       </c>
       <c r="D69" t="s">
         <v>378</v>
       </c>
       <c r="E69" t="str">
-        <f>RIGHT(D69,LEN(D69)-FIND("Line ",D69)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 3102</v>
       </c>
       <c r="F69" t="str">
-        <f>LEFT(D69,LEN(D69)-LEN(E69))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.UIElement.OnMouseLeftButtonUpThunk(object sender, System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
       <c r="G69" t="str">
-        <f>LEFT(F69,FIND("(",F69))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.UIElement.OnMouseLeftButtonUpThunk(</v>
       </c>
       <c r="H69">
-        <f>FIND("@",SUBSTITUTE(G69,".","@",LEN(G69)-LEN(SUBSTITUTE(G69,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>46</v>
       </c>
       <c r="I69" t="str">
-        <f>RIGHT(F69,LEN(F69)-H69)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">OnMouseLeftButtonUpThunk(object sender, System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>70</v>
       </c>
       <c r="C70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>70</v>
       </c>
       <c r="D70" t="s">
         <v>379</v>
       </c>
       <c r="E70" t="str">
-        <f>RIGHT(D70,LEN(D70)-FIND("Line ",D70)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 98</v>
       </c>
       <c r="F70" t="str">
-        <f>LEFT(D70,LEN(D70)-LEN(E70))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.Input.MouseButtonEventArgs.InvokeEventHandler(System.Delegate genericHandler, object genericTarget) </v>
       </c>
       <c r="G70" t="str">
-        <f>LEFT(F70,FIND("(",F70))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.Input.MouseButtonEventArgs.InvokeEventHandler(</v>
       </c>
       <c r="H70">
-        <f>FIND("@",SUBSTITUTE(G70,".","@",LEN(G70)-LEN(SUBSTITUTE(G70,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>63</v>
       </c>
       <c r="I70" t="str">
-        <f>RIGHT(F70,LEN(F70)-H70)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeEventHandler(System.Delegate genericHandler, object genericTarget) </v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>71</v>
       </c>
       <c r="C71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>71</v>
       </c>
       <c r="D71" t="s">
         <v>43</v>
       </c>
       <c r="E71" t="str">
-        <f>RIGHT(D71,LEN(D71)-FIND("Line ",D71)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 190</v>
       </c>
       <c r="F71" t="str">
-        <f>LEFT(D71,LEN(D71)-LEN(E71))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.RoutedEventArgs.InvokeHandler(System.Delegate handler, object target) </v>
       </c>
       <c r="G71" t="str">
-        <f>LEFT(F71,FIND("(",F71))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.RoutedEventArgs.InvokeHandler(</v>
       </c>
       <c r="H71">
-        <f>FIND("@",SUBSTITUTE(G71,".","@",LEN(G71)-LEN(SUBSTITUTE(G71,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>52</v>
       </c>
       <c r="I71" t="str">
-        <f>RIGHT(F71,LEN(F71)-H71)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandler(System.Delegate handler, object target) </v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>72</v>
       </c>
       <c r="C72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>72</v>
       </c>
       <c r="D72" t="s">
         <v>44</v>
       </c>
       <c r="E72" t="str">
-        <f>RIGHT(D72,LEN(D72)-FIND("Line ",D72)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 66</v>
       </c>
       <c r="F72" t="str">
-        <f>LEFT(D72,LEN(D72)-LEN(E72))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
       <c r="G72" t="str">
-        <f>LEFT(F72,FIND("(",F72))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(</v>
       </c>
       <c r="H72">
-        <f>FIND("@",SUBSTITUTE(G72,".","@",LEN(G72)-LEN(SUBSTITUTE(G72,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>59</v>
       </c>
       <c r="I72" t="str">
-        <f>RIGHT(F72,LEN(F72)-H72)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>73</v>
       </c>
       <c r="C73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>73</v>
       </c>
       <c r="D73" t="s">
         <v>38</v>
       </c>
       <c r="E73" t="str">
-        <f>RIGHT(D73,LEN(D73)-FIND("Line ",D73)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 103</v>
       </c>
       <c r="F73" t="str">
-        <f>LEFT(D73,LEN(D73)-LEN(E73))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
       <c r="G73" t="str">
-        <f>LEFT(F73,FIND("(",F73))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(</v>
       </c>
       <c r="H73">
-        <f>FIND("@",SUBSTITUTE(G73,".","@",LEN(G73)-LEN(SUBSTITUTE(G73,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>47</v>
       </c>
       <c r="I73" t="str">
-        <f>RIGHT(F73,LEN(F73)-H73)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>74</v>
       </c>
       <c r="C74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>74</v>
       </c>
       <c r="D74" t="s">
         <v>45</v>
       </c>
       <c r="E74" t="str">
-        <f>RIGHT(D74,LEN(D74)-FIND("Line ",D74)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 6078</v>
       </c>
       <c r="F74" t="str">
-        <f>LEFT(D74,LEN(D74)-LEN(E74))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.UIElement.ReRaiseEventAs(System.Windows.DependencyObject sender, System.Windows.RoutedEventArgs args, System.Windows.RoutedEvent newEvent) </v>
       </c>
       <c r="G74" t="str">
-        <f>LEFT(F74,FIND("(",F74))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.UIElement.ReRaiseEventAs(</v>
       </c>
       <c r="H74">
-        <f>FIND("@",SUBSTITUTE(G74,".","@",LEN(G74)-LEN(SUBSTITUTE(G74,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>46</v>
       </c>
       <c r="I74" t="str">
-        <f>RIGHT(F74,LEN(F74)-H74)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">ReRaiseEventAs(System.Windows.DependencyObject sender, System.Windows.RoutedEventArgs args, System.Windows.RoutedEvent newEvent) </v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>75</v>
       </c>
       <c r="C75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>75</v>
       </c>
       <c r="D75" t="s">
         <v>46</v>
       </c>
       <c r="E75" t="str">
-        <f>RIGHT(D75,LEN(D75)-FIND("Line ",D75)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 3027</v>
       </c>
       <c r="F75" t="str">
-        <f>LEFT(D75,LEN(D75)-LEN(E75))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.UIElement.OnMouseUpThunk(object sender, System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
       <c r="G75" t="str">
-        <f>LEFT(F75,FIND("(",F75))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.UIElement.OnMouseUpThunk(</v>
       </c>
       <c r="H75">
-        <f>FIND("@",SUBSTITUTE(G75,".","@",LEN(G75)-LEN(SUBSTITUTE(G75,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>46</v>
       </c>
       <c r="I75" t="str">
-        <f>RIGHT(F75,LEN(F75)-H75)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">OnMouseUpThunk(object sender, System.Windows.Input.MouseButtonEventArgs e) </v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>76</v>
       </c>
       <c r="C76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>76</v>
       </c>
       <c r="D76" t="s">
         <v>379</v>
       </c>
       <c r="E76" t="str">
-        <f>RIGHT(D76,LEN(D76)-FIND("Line ",D76)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 98</v>
       </c>
       <c r="F76" t="str">
-        <f>LEFT(D76,LEN(D76)-LEN(E76))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.Input.MouseButtonEventArgs.InvokeEventHandler(System.Delegate genericHandler, object genericTarget) </v>
       </c>
       <c r="G76" t="str">
-        <f>LEFT(F76,FIND("(",F76))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.Input.MouseButtonEventArgs.InvokeEventHandler(</v>
       </c>
       <c r="H76">
-        <f>FIND("@",SUBSTITUTE(G76,".","@",LEN(G76)-LEN(SUBSTITUTE(G76,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>63</v>
       </c>
       <c r="I76" t="str">
-        <f>RIGHT(F76,LEN(F76)-H76)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeEventHandler(System.Delegate genericHandler, object genericTarget) </v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>77</v>
       </c>
       <c r="C77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>77</v>
       </c>
       <c r="D77" t="s">
         <v>43</v>
       </c>
       <c r="E77" t="str">
-        <f>RIGHT(D77,LEN(D77)-FIND("Line ",D77)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 190</v>
       </c>
       <c r="F77" t="str">
-        <f>LEFT(D77,LEN(D77)-LEN(E77))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.RoutedEventArgs.InvokeHandler(System.Delegate handler, object target) </v>
       </c>
       <c r="G77" t="str">
-        <f>LEFT(F77,FIND("(",F77))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.RoutedEventArgs.InvokeHandler(</v>
       </c>
       <c r="H77">
-        <f>FIND("@",SUBSTITUTE(G77,".","@",LEN(G77)-LEN(SUBSTITUTE(G77,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>52</v>
       </c>
       <c r="I77" t="str">
-        <f>RIGHT(F77,LEN(F77)-H77)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandler(System.Delegate handler, object target) </v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>78</v>
       </c>
       <c r="C78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>78</v>
       </c>
       <c r="D78" t="s">
         <v>44</v>
       </c>
       <c r="E78" t="str">
-        <f>RIGHT(D78,LEN(D78)-FIND("Line ",D78)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 66</v>
       </c>
       <c r="F78" t="str">
-        <f>LEFT(D78,LEN(D78)-LEN(E78))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
       <c r="G78" t="str">
-        <f>LEFT(F78,FIND("(",F78))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.RoutedEventHandlerInfo.InvokeHandler(</v>
       </c>
       <c r="H78">
-        <f>FIND("@",SUBSTITUTE(G78,".","@",LEN(G78)-LEN(SUBSTITUTE(G78,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>59</v>
       </c>
       <c r="I78" t="str">
-        <f>RIGHT(F78,LEN(F78)-H78)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandler(object target, System.Windows.RoutedEventArgs routedEventArgs) </v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>79</v>
       </c>
       <c r="C79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>79</v>
       </c>
       <c r="D79" t="s">
         <v>38</v>
       </c>
       <c r="E79" t="str">
-        <f>RIGHT(D79,LEN(D79)-FIND("Line ",D79)+1)</f>
+        <f t="shared" si="12"/>
         <v>Line 103</v>
       </c>
       <c r="F79" t="str">
-        <f>LEFT(D79,LEN(D79)-LEN(E79))</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
       <c r="G79" t="str">
-        <f>LEFT(F79,FIND("(",F79))</f>
+        <f t="shared" si="14"/>
         <v>PresentationCore.dll!System.Windows.EventRoute.InvokeHandlersImpl(</v>
       </c>
       <c r="H79">
-        <f>FIND("@",SUBSTITUTE(G79,".","@",LEN(G79)-LEN(SUBSTITUTE(G79,".",""))))</f>
+        <f t="shared" si="15"/>
         <v>47</v>
       </c>
       <c r="I79" t="str">
-        <f>RIGHT(F79,LEN(F79)-H79)</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">InvokeHandlersImpl(object source, System.Windows.RoutedEventArgs args, bool reRaised) </v>
       </c>
     </row>
@@ -11190,12 +11059,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E79">
-    <cfRule type="containsErrors" dxfId="4" priority="7">
+    <cfRule type="containsErrors" dxfId="5" priority="7">
       <formula>ISERROR(E1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F79">
-    <cfRule type="containsErrors" dxfId="0" priority="1">
+    <cfRule type="containsErrors" dxfId="4" priority="1">
       <formula>ISERROR(F1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11227,12 +11096,6 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="2">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>